<commit_message>
Creating of folder.  Combining Use Cases.  Also edited by Lerato.
</commit_message>
<xml_diff>
--- a/COS301Phase1/UseCases/UseCases.xlsx
+++ b/COS301Phase1/UseCases/UseCases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohannDian\Desktop\301Project\phase1\COS301Phase1\Use Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohannDian\Desktop\301P\New\COS301Phase1\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>Use Case</t>
   </si>
@@ -151,9 +150,6 @@
     <t>Checked if user is allowed to perform the chosen function/see the chosen thread.  If user hirarchy allows for chosen function to be carried out, perform function.  If user is not in the correct social group, deny access, return exception, do not show post and show an error message on screen.</t>
   </si>
   <si>
-    <t>Create own post(c)</t>
-  </si>
-  <si>
     <r>
       <t>·</t>
     </r>
@@ -372,12 +368,27 @@
   <si>
     <t>User must be registered. User must be of type(Lecturer/Student/TA) that is acceptable to be promoted. User must have enough participation points to be changed to the next level.</t>
   </si>
+  <si>
+    <t>User creates a post on the the buzzSpace. (l)</t>
+  </si>
+  <si>
+    <t>create post</t>
+  </si>
+  <si>
+    <t>user reads a post on the buzzSpace</t>
+  </si>
+  <si>
+    <t>user edits and then update a post on the buzzSpace.</t>
+  </si>
+  <si>
+    <t>User can delete its own post.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -414,13 +425,6 @@
       <sz val="26"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -598,10 +602,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -950,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -983,92 +987,100 @@
     </row>
     <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="10"/>
+        <v>43</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>72</v>
+      </c>
       <c r="D6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>73</v>
+      </c>
       <c r="D7" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -1076,14 +1088,14 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="63" x14ac:dyDescent="0.25">
@@ -1095,10 +1107,10 @@
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -1153,13 +1165,13 @@
         <v>9</v>
       </c>
       <c r="C16" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="E16" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
@@ -1204,13 +1216,13 @@
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="236.25" x14ac:dyDescent="0.25">

</xml_diff>